<commit_message>
Updates for GTEX/TCGA example
</commit_message>
<xml_diff>
--- a/fasp/runner/credits/ScriptSummary.xlsx
+++ b/fasp/runner/credits/ScriptSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forei/dev/fasp-scripts/fasp/runner/credits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE818F9-B355-6747-A1C2-F4E59ECACBDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DA241-E208-564C-A9F7-892EB7AB252C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="3660" windowWidth="45340" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="3660" windowWidth="45340" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pipelineLog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>script</t>
   </si>
@@ -203,6 +203,21 @@
   </si>
   <si>
     <t>SRAExample</t>
+  </si>
+  <si>
+    <t>FASPScript18.py</t>
+  </si>
+  <si>
+    <t>sbWESClient</t>
+  </si>
+  <si>
+    <t>Anvil GTEX SB</t>
+  </si>
+  <si>
+    <t>Modified version of 15 to use free amazon data. Move to notebook</t>
+  </si>
+  <si>
+    <t>Gen3ManifestClient</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G26"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1141,7 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="60.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="65" customHeight="1" x14ac:dyDescent="0.3">
@@ -1496,72 +1511,93 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="10"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="2" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
+    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E21">
-    <sortCondition ref="A3:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E22">
+    <sortCondition ref="A3:A22"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Scripts to notebooks and pruning
</commit_message>
<xml_diff>
--- a/fasp/runner/credits/ScriptSummary.xlsx
+++ b/fasp/runner/credits/ScriptSummary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forei/dev/fasp-scripts/fasp/runner/credits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DA241-E208-564C-A9F7-892EB7AB252C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C7AE1-FC52-8243-9947-8C94F1C7D1B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="3660" windowWidth="45340" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>script</t>
   </si>
@@ -181,24 +181,15 @@
     <t>GTEx and TCGA</t>
   </si>
   <si>
-    <t>Retire</t>
-  </si>
-  <si>
     <t>Notebook done</t>
   </si>
   <si>
     <t>FASPScript16.py</t>
   </si>
   <si>
-    <t>Replace with SRA DRS</t>
-  </si>
-  <si>
     <t>Notebook and use Seven Bridges WES</t>
   </si>
   <si>
-    <t>Notebook and use Seven Bridges WES, demo use of two stacks</t>
-  </si>
-  <si>
     <t>retire - 14 is preferable</t>
   </si>
   <si>
@@ -218,13 +209,76 @@
   </si>
   <si>
     <t>Gen3ManifestClient</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>FASPNotebook09</t>
+  </si>
+  <si>
+    <t>FASPNotebook10</t>
+  </si>
+  <si>
+    <t>FASPNotebook02</t>
+  </si>
+  <si>
+    <t>Retire - had value as a step on the way to 4</t>
+  </si>
+  <si>
+    <t>In terms of a 'full house' superseded by other notebooks, but has value in that uses the DNAStack WES client. In the move to notebooks many scripts have been adapted to use the SB client in place of DNA Stack or direct GCP compute.</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Same query as in 2, uses SB compute instead of GCP.</t>
+  </si>
+  <si>
+    <t>Move to notebook</t>
+  </si>
+  <si>
+    <t>SDL now superseded by SRA DRS. Has value in that MD5 returns an output as part of the response. As opposed to just a file</t>
+  </si>
+  <si>
+    <t>Move to notebook. Demonstrate return of the result into a dataframe.</t>
+  </si>
+  <si>
+    <t>Value is in using a user originated scientific question. Can be moved to a full house using DiscovertSearchClient and an SB compute.</t>
+  </si>
+  <si>
+    <t>Value as validation for 9</t>
+  </si>
+  <si>
+    <t>Different dataset (GECCO), controlled access dataset</t>
+  </si>
+  <si>
+    <t>Needs dataset with index files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notebook done and moved to full house. </t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Request access to provided dataset</t>
+  </si>
+  <si>
+    <t>GTEX Example</t>
+  </si>
+  <si>
+    <t>Replace with SRA DRS. Companion to 15. Same notebook?</t>
+  </si>
+  <si>
+    <t>Notebook done and use Seven Bridges WES, demo use of two stacks, and double up FASPRunner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,6 +435,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -575,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -705,6 +772,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -750,7 +863,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -772,6 +885,50 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1128,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G27"/>
+  <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+      <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,10 +1298,11 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="60.1640625" customWidth="1"/>
+    <col min="6" max="6" width="86.1640625" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1160,8 +1318,14 @@
       <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1178,11 +1342,11 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1198,10 +1362,14 @@
       <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="8"/>
@@ -1209,10 +1377,11 @@
         <v>14</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F5" s="15"/>
+      <c r="G5" s="19"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1229,11 +1398,11 @@
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="100" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1249,10 +1418,14 @@
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F7" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1268,173 +1441,192 @@
       <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="50" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="F11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F12" s="19"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>59</v>
+        <v>77</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>8</v>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>46</v>
@@ -1442,35 +1634,36 @@
       <c r="E17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>60</v>
+      <c r="F17" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>49</v>
@@ -1478,127 +1671,178 @@
       <c r="C19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
+      <c r="D19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>41</v>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>63</v>
+      <c r="A21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
       <c r="D23" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="1" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E22">
-    <sortCondition ref="A3:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E24">
+    <sortCondition ref="A3:A24"/>
   </sortState>
-  <mergeCells count="12">
-    <mergeCell ref="E26:E27"/>
+  <mergeCells count="24">
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
   </mergeCells>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CDS Examples, JMJD1C on GA4GH Search
</commit_message>
<xml_diff>
--- a/fasp/runner/credits/ScriptSummary.xlsx
+++ b/fasp/runner/credits/ScriptSummary.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forei/dev/fasp-scripts/fasp/runner/credits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C7AE1-FC52-8243-9947-8C94F1C7D1B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3C99F-5C4E-FE4A-9422-D4DE27235034}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3660" windowWidth="45340" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30460" yWindow="460" windowWidth="37380" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pipelineLog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -232,9 +243,6 @@
     <t>To do</t>
   </si>
   <si>
-    <t>Same query as in 2, uses SB compute instead of GCP.</t>
-  </si>
-  <si>
     <t>Move to notebook</t>
   </si>
   <si>
@@ -272,6 +280,9 @@
   </si>
   <si>
     <t>Notebook done and use Seven Bridges WES, demo use of two stacks, and double up FASPRunner</t>
+  </si>
+  <si>
+    <t>Same query as in 2, uses SB compute instead of GCP. Retire as Notebook02 now does SB compute</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1299,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D12"/>
+      <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>63</v>
@@ -1425,7 +1436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="50" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1441,8 +1452,8 @@
       <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>70</v>
+      <c r="F8" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -1463,10 +1474,10 @@
         <v>9</v>
       </c>
       <c r="F9" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="50" x14ac:dyDescent="0.3">
@@ -1486,10 +1497,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -1509,10 +1520,10 @@
         <v>22</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -1589,10 +1600,10 @@
         <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -1612,10 +1623,10 @@
         <v>6</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.3">
@@ -1655,7 +1666,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>57</v>
@@ -1681,7 +1692,7 @@
         <v>55</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.3">
@@ -1701,7 +1712,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1722,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Pre Connect March 21
</commit_message>
<xml_diff>
--- a/fasp/runner/credits/ScriptSummary.xlsx
+++ b/fasp/runner/credits/ScriptSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/forei/dev/fasp-scripts/fasp/runner/credits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E3C99F-5C4E-FE4A-9422-D4DE27235034}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBEC9BF-E605-374D-85E3-3FE6D23EED88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30460" yWindow="460" windowWidth="37380" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33500" yWindow="460" windowWidth="37860" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pipelineLog" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
   <si>
     <t>script</t>
   </si>
@@ -240,9 +240,6 @@
     <t>In terms of a 'full house' superseded by other notebooks, but has value in that uses the DNAStack WES client. In the move to notebooks many scripts have been adapted to use the SB client in place of DNA Stack or direct GCP compute.</t>
   </si>
   <si>
-    <t>To do</t>
-  </si>
-  <si>
     <t>Move to notebook</t>
   </si>
   <si>
@@ -261,21 +258,12 @@
     <t>Different dataset (GECCO), controlled access dataset</t>
   </si>
   <si>
-    <t>Needs dataset with index files</t>
-  </si>
-  <si>
     <t xml:space="preserve">Notebook done and moved to full house. </t>
   </si>
   <si>
     <t>Discussion</t>
   </si>
   <si>
-    <t>Request access to provided dataset</t>
-  </si>
-  <si>
-    <t>GTEX Example</t>
-  </si>
-  <si>
     <t>Replace with SRA DRS. Companion to 15. Same notebook?</t>
   </si>
   <si>
@@ -283,6 +271,24 @@
   </si>
   <si>
     <t>Same query as in 2, uses SB compute instead of GCP. Retire as Notebook02 now does SB compute</t>
+  </si>
+  <si>
+    <t>Needs dataset with index files. Request access to provided dataset.</t>
+  </si>
+  <si>
+    <t>FASPNotebook12</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Needs to run on cloud vm</t>
+  </si>
+  <si>
+    <t>FASPNotebook15-GTEXExample-GCP</t>
+  </si>
+  <si>
+    <t>FASPNotebook18-GTEXExample-AWS</t>
   </si>
 </sst>
 </file>
@@ -882,6 +888,50 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,50 +946,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1299,7 +1305,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1329,10 +1335,10 @@
       <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1356,41 +1362,47 @@
         <v>67</v>
       </c>
       <c r="G3" s="3"/>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="26" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="21" t="s">
         <v>66</v>
       </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="19"/>
-      <c r="K5" s="17"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="22"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1429,11 +1441,11 @@
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="9" t="s">
         <v>68</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="50" x14ac:dyDescent="0.3">
@@ -1452,10 +1464,13 @@
       <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>83</v>
+      <c r="F8" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="G8" s="3"/>
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -1464,20 +1479,20 @@
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="50" x14ac:dyDescent="0.3">
@@ -1487,55 +1502,55 @@
       <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>70</v>
+      <c r="F10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="23" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>70</v>
+      <c r="F11" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="24"/>
       <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1600,10 +1615,10 @@
         <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -1623,10 +1638,10 @@
         <v>6</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="24" x14ac:dyDescent="0.3">
@@ -1666,7 +1681,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>57</v>
@@ -1691,8 +1706,8 @@
       <c r="F19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="27" t="s">
-        <v>80</v>
+      <c r="G19" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.3">
@@ -1712,15 +1727,15 @@
         <v>6</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1729,28 +1744,28 @@
       <c r="D21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="12" t="s">
+      <c r="F21" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -1771,75 +1786,65 @@
       <c r="F23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="28" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E24">
     <sortCondition ref="A3:A24"/>
   </sortState>
   <mergeCells count="24">
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E4:E5"/>
@@ -1852,6 +1857,18 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>